<commit_message>
1) Factored out Bing and Google Translators 2) Updated settings.json to dynamically add translators 3) add python logging 4) Updated Readme.md
</commit_message>
<xml_diff>
--- a/translate-helper/data/output_data.xlsx
+++ b/translate-helper/data/output_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="83">
   <si>
     <t>Word</t>
   </si>
@@ -22,10 +22,7 @@
     <t>Category</t>
   </si>
   <si>
-    <t>GoogleTranslation</t>
-  </si>
-  <si>
-    <t>BingTranslation</t>
+    <t>Google Translator</t>
   </si>
   <si>
     <t>Watermelon</t>
@@ -266,60 +263,6 @@
   </si>
   <si>
     <t>طول و عرض</t>
-  </si>
-  <si>
-    <t>واٹرمیلاون</t>
-  </si>
-  <si>
-    <t>واٹیرمیلاون</t>
-  </si>
-  <si>
-    <t>بیر</t>
-  </si>
-  <si>
-    <t>پرسامماون</t>
-  </si>
-  <si>
-    <t>پرساماون</t>
-  </si>
-  <si>
-    <t>گواوا</t>
-  </si>
-  <si>
-    <t>پپیتے</t>
-  </si>
-  <si>
-    <t>ایپل</t>
-  </si>
-  <si>
-    <t>آلو بالو</t>
-  </si>
-  <si>
-    <t>آم کے چھلکے کو</t>
-  </si>
-  <si>
-    <t>آلسپاﺋیس</t>
-  </si>
-  <si>
-    <t>سر کرنا</t>
-  </si>
-  <si>
-    <t>لوکی</t>
-  </si>
-  <si>
-    <t>مارچوبہ</t>
-  </si>
-  <si>
-    <t>بیٹروٹ</t>
-  </si>
-  <si>
-    <t>شاخ گوبھی</t>
-  </si>
-  <si>
-    <t>بند گوبھی</t>
-  </si>
-  <si>
-    <t>شملہ مرچ</t>
   </si>
 </sst>
 </file>
@@ -677,13 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,824 +636,677 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
-      </c>
-      <c r="E43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>